<commit_message>
Update Certification Tracker Public.xlsx
</commit_message>
<xml_diff>
--- a/Resume Resources/Certifications/Certification Tracker Public.xlsx
+++ b/Resume Resources/Certifications/Certification Tracker Public.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6917bc646511f86f/Coraline/Resume Resources/Certifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A925435C-02FC-F249-A13E-999138065F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7064019-5010-7141-B0D9-94A277D8299D}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{A925435C-02FC-F249-A13E-999138065F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB40754-88C2-7241-B01D-AB872FD1D2B5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="266">
   <si>
     <t>My Certifications</t>
   </si>
@@ -6677,7 +6677,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6861,7 +6861,9 @@
       <c r="G3" s="36" t="s">
         <v>240</v>
       </c>
-      <c r="H3" s="90"/>
+      <c r="H3" s="90" t="s">
+        <v>126</v>
+      </c>
       <c r="I3" s="91">
         <v>44806</v>
       </c>

</xml_diff>